<commit_message>
feat:log sync speed pre image
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daijun/Desktop/GeminiTopProject/image-offline-sync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daijun/Desktop/GeminiTopProject/image-sync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4537CC-674C-3B41-97DC-07366B79620F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11CAF20-DFD2-D74C-9FD7-9E6083A3C746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="6680" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>image_id</t>
   </si>
@@ -52,34 +52,48 @@
     <t>11821</t>
   </si>
   <si>
-    <t>njnonpry6rws/1-20230823165944</t>
-  </si>
-  <si>
-    <t>njnonpry6rws/1-20230823170035</t>
-  </si>
-  <si>
-    <t>20230823170035</t>
-  </si>
-  <si>
-    <t>20230823165944</t>
-  </si>
-  <si>
-    <t>miniconda3</t>
-  </si>
-  <si>
-    <t>uxemqox7pw6n/nvcr.io</t>
+    <t>11822</t>
+  </si>
+  <si>
+    <t>11823</t>
+  </si>
+  <si>
+    <t>11.1-tensorflow1.15.4-py3-nvcr.io</t>
+  </si>
+  <si>
+    <t>11.0.3-tensorflow2.4.3-pytorch1.7.1-py3.8-cudnn8-devel-ubuntu20.04</t>
+  </si>
+  <si>
+    <t>11.2.2-tensorflow2.5.0-py3.8-cudnn8-devel-ubuntu20.04</t>
+  </si>
+  <si>
+    <t>11.3.1-pytorch1.12.1-py3.8-cudnn8-devel-ubuntu20.04</t>
+  </si>
+  <si>
+    <t>11.3.1-pytorch1.11.0-py3.8-cudnn8-devel-ubuntu20.04</t>
+  </si>
+  <si>
+    <t>nvidia/cuda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -103,12 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -445,20 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,49 +485,78 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1 B1:C1" numberStoredAsText="1"/>

</xml_diff>